<commit_message>
Input has now nested wishes
The nested wishes are following participant's wishes: Julius Kuusisto, Alina Tamminen. So in main excel if wishes are NOT forced to be mutual the participants who's surname is Kuusisto, Laurila or Tammila should be shown to belown to the same group.
</commit_message>
<xml_diff>
--- a/input-participant-and_wishing-list.xlsx
+++ b/input-participant-and_wishing-list.xlsx
@@ -823,7 +823,7 @@
     <t xml:space="preserve">Julius Kuusisto</t>
   </si>
   <si>
-    <t xml:space="preserve">Kim Kuusisto, Kati Kuusisto, Margareta Kuusisto, Topi Kuusisto</t>
+    <t xml:space="preserve">Kim Kuusisto, Kati Kuusisto, Margareta Kuusisto, Topi Kuusisto, Tanja Laurila</t>
   </si>
   <si>
     <t xml:space="preserve">Margareta Kuusisto</t>
@@ -841,7 +841,7 @@
     <t xml:space="preserve">Alina Tamminen</t>
   </si>
   <si>
-    <t xml:space="preserve">Johan Tamminen, Elli Tamminen, Konsta Tamminen, Marja-Liisa Tamminen</t>
+    <t xml:space="preserve">Johan Tamminen, Elli Tamminen, Konsta Tamminen, Marja-Liisa Tamminen, Topi Kuusisto</t>
   </si>
   <si>
     <t xml:space="preserve">Johan Tamminen</t>
@@ -968,10 +968,10 @@
   <dimension ref="A1:C142"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A118" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C141" activeCellId="0" sqref="C141"/>
+      <selection pane="topLeft" activeCell="C135" activeCellId="0" sqref="C135"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.12"/>

</xml_diff>

<commit_message>
Updated examples to mutual group outside mutual pool
</commit_message>
<xml_diff>
--- a/input-participant-and_wishing-list.xlsx
+++ b/input-participant-and_wishing-list.xlsx
@@ -283,7 +283,7 @@
     <t xml:space="preserve">Martti Koivisto</t>
   </si>
   <si>
-    <t xml:space="preserve">Pertti Koivisto, Laura Koivisto, Elisabet Koivisto, Reijo Koivisto</t>
+    <t xml:space="preserve">Pertti Koivisto, Laura Koivisto, Elisabet Koivisto, Reijo Koivisto, Satu Räsänen</t>
   </si>
   <si>
     <t xml:space="preserve">Elisabet Koivisto</t>
@@ -301,7 +301,7 @@
     <t xml:space="preserve">Satu Räsänen</t>
   </si>
   <si>
-    <t xml:space="preserve">Tuomas Räsänen, Mari Räsänen, Olli Räsänen, Heidi Räsänen</t>
+    <t xml:space="preserve">Tuomas Räsänen, Mari Räsänen, Olli Räsänen, Heidi Räsänen, Martti Koivisto</t>
   </si>
   <si>
     <t xml:space="preserve">Tuomas Räsänen</t>
@@ -811,7 +811,7 @@
     <t xml:space="preserve">Kim Kuusisto</t>
   </si>
   <si>
-    <t xml:space="preserve">Kati Kuusisto, Julius Kuusisto, Margareta Kuusisto, Topi Kuusisto</t>
+    <t xml:space="preserve">Kati Kuusisto, Julius Kuusisto, Margareta Kuusisto, Topi Kuusisto, Elli Tamminen</t>
   </si>
   <si>
     <t xml:space="preserve">Kati Kuusisto</t>
@@ -835,7 +835,7 @@
     <t xml:space="preserve">Topi Kuusisto</t>
   </si>
   <si>
-    <t xml:space="preserve">Kim Kuusisto, Kati Kuusisto, Julius Kuusisto, Margareta Kuusisto</t>
+    <t xml:space="preserve">Kim Kuusisto, Kati Kuusisto, Julius Kuusisto, Margareta Kuusisto, Alina Tamminen</t>
   </si>
   <si>
     <t xml:space="preserve">Alina Tamminen</t>
@@ -853,7 +853,7 @@
     <t xml:space="preserve">Elli Tamminen</t>
   </si>
   <si>
-    <t xml:space="preserve">Alina Tamminen, Johan Tamminen, Konsta Tamminen, Marja-Liisa Tamminen</t>
+    <t xml:space="preserve">Alina Tamminen, Johan Tamminen, Konsta Tamminen, Marja-Liisa Tamminen, Kim Kuusisto, toimisko tämä?</t>
   </si>
   <si>
     <t xml:space="preserve">Konsta Tamminen</t>
@@ -967,11 +967,11 @@
   </sheetPr>
   <dimension ref="A1:C142"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A118" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C135" activeCellId="0" sqref="C135"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A109" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C139" activeCellId="0" sqref="C139"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.12"/>

</xml_diff>

<commit_message>
Updated output and input excel
</commit_message>
<xml_diff>
--- a/input-participant-and_wishing-list.xlsx
+++ b/input-participant-and_wishing-list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="289">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -823,7 +823,7 @@
     <t xml:space="preserve">Julius Kuusisto</t>
   </si>
   <si>
-    <t xml:space="preserve">Kim Kuusisto, Kati Kuusisto, Margareta Kuusisto, Topi Kuusisto, Tanja Laurila</t>
+    <t xml:space="preserve">Kim Kuusisto, Kati Kuusisto, Margareta Kuusisto, Topi Kuusisto, Tanja Laurila, Alina Tamminen</t>
   </si>
   <si>
     <t xml:space="preserve">Margareta Kuusisto</t>
@@ -841,7 +841,7 @@
     <t xml:space="preserve">Alina Tamminen</t>
   </si>
   <si>
-    <t xml:space="preserve">Johan Tamminen, Elli Tamminen, Konsta Tamminen, Marja-Liisa Tamminen, Topi Kuusisto</t>
+    <t xml:space="preserve">Johan Tamminen, Elli Tamminen, Konsta Tamminen, Marja-Liisa Tamminen, Topi Kuusisto, Julius Kuusisto</t>
   </si>
   <si>
     <t xml:space="preserve">Johan Tamminen</t>
@@ -869,6 +869,24 @@
   </si>
   <si>
     <t xml:space="preserve">Akseli Karhu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b, d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a, c</t>
   </si>
 </sst>
 </file>
@@ -965,13 +983,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C142"/>
+  <dimension ref="A1:C146"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A109" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C139" activeCellId="0" sqref="C139"/>
+      <selection pane="topLeft" activeCell="C132" activeCellId="0" sqref="C132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.12"/>
@@ -2532,6 +2550,38 @@
       </c>
       <c r="B142" s="0" t="s">
         <v>282</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B143" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="C143" s="0" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B144" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="C144" s="0" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B145" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="C145" s="0" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B146" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="C146" s="0" t="s">
+        <v>288</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Input with some new participants
</commit_message>
<xml_diff>
--- a/input-participant-and_wishing-list.xlsx
+++ b/input-participant-and_wishing-list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="291">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -853,7 +853,7 @@
     <t xml:space="preserve">Elli Tamminen</t>
   </si>
   <si>
-    <t xml:space="preserve">Alina Tamminen, Johan Tamminen, Konsta Tamminen, Marja-Liisa Tamminen, Kim Kuusisto, toimisko tämä?</t>
+    <t xml:space="preserve">Alina Tamminen, Johan Tamminen, Konsta Tamminen, Marja-Liisa Tamminen, Kim Kuusisto</t>
   </si>
   <si>
     <t xml:space="preserve">Konsta Tamminen</t>
@@ -887,6 +887,12 @@
   </si>
   <si>
     <t xml:space="preserve">a, c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">w</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asdasdasd</t>
   </si>
 </sst>
 </file>
@@ -983,13 +989,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C146"/>
+  <dimension ref="A1:C147"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A109" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C132" activeCellId="0" sqref="C132"/>
+      <selection pane="topLeft" activeCell="C139" activeCellId="0" sqref="C139"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.12"/>
@@ -2582,6 +2588,14 @@
       </c>
       <c r="C146" s="0" t="s">
         <v>288</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B147" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="C147" s="0" t="s">
+        <v>290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed indexing, since it broke the code if there was index and no name
- Broke if there was a index and not name next to index. Not sure why that broke the code, but will be fixed in at a later date
</commit_message>
<xml_diff>
--- a/input-participant-and_wishing-list.xlsx
+++ b/input-participant-and_wishing-list.xlsx
@@ -989,13 +989,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C147"/>
+  <dimension ref="B1:C147"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A109" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C139" activeCellId="0" sqref="C139"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.12"/>
@@ -1011,9 +1011,6 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>0</v>
-      </c>
       <c r="B2" s="0" t="s">
         <v>2</v>
       </c>
@@ -1022,9 +1019,6 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>1</v>
-      </c>
       <c r="B3" s="0" t="s">
         <v>4</v>
       </c>
@@ -1033,9 +1027,6 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>2</v>
-      </c>
       <c r="B4" s="0" t="s">
         <v>6</v>
       </c>
@@ -1044,9 +1035,6 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>3</v>
-      </c>
       <c r="B5" s="0" t="s">
         <v>8</v>
       </c>
@@ -1055,9 +1043,6 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>4</v>
-      </c>
       <c r="B6" s="0" t="s">
         <v>10</v>
       </c>
@@ -1066,9 +1051,6 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>5</v>
-      </c>
       <c r="B7" s="0" t="s">
         <v>12</v>
       </c>
@@ -1077,9 +1059,6 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>6</v>
-      </c>
       <c r="B8" s="0" t="s">
         <v>14</v>
       </c>
@@ -1088,9 +1067,6 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>7</v>
-      </c>
       <c r="B9" s="0" t="s">
         <v>16</v>
       </c>
@@ -1099,9 +1075,6 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>8</v>
-      </c>
       <c r="B10" s="0" t="s">
         <v>18</v>
       </c>
@@ -1110,9 +1083,6 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
-        <v>9</v>
-      </c>
       <c r="B11" s="0" t="s">
         <v>20</v>
       </c>
@@ -1121,9 +1091,6 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>10</v>
-      </c>
       <c r="B12" s="0" t="s">
         <v>22</v>
       </c>
@@ -1132,9 +1099,6 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
-        <v>11</v>
-      </c>
       <c r="B13" s="0" t="s">
         <v>24</v>
       </c>
@@ -1143,9 +1107,6 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
-        <v>12</v>
-      </c>
       <c r="B14" s="0" t="s">
         <v>26</v>
       </c>
@@ -1154,9 +1115,6 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
-        <v>13</v>
-      </c>
       <c r="B15" s="0" t="s">
         <v>28</v>
       </c>
@@ -1165,9 +1123,6 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
-        <v>14</v>
-      </c>
       <c r="B16" s="0" t="s">
         <v>30</v>
       </c>
@@ -1176,9 +1131,6 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
-        <v>15</v>
-      </c>
       <c r="B17" s="0" t="s">
         <v>32</v>
       </c>
@@ -1187,9 +1139,6 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
-        <v>16</v>
-      </c>
       <c r="B18" s="0" t="s">
         <v>34</v>
       </c>
@@ -1198,9 +1147,6 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
-        <v>17</v>
-      </c>
       <c r="B19" s="0" t="s">
         <v>36</v>
       </c>
@@ -1209,9 +1155,6 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
-        <v>18</v>
-      </c>
       <c r="B20" s="0" t="s">
         <v>38</v>
       </c>
@@ -1220,9 +1163,6 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
-        <v>19</v>
-      </c>
       <c r="B21" s="0" t="s">
         <v>40</v>
       </c>
@@ -1231,9 +1171,6 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
-        <v>20</v>
-      </c>
       <c r="B22" s="0" t="s">
         <v>42</v>
       </c>
@@ -1242,9 +1179,6 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
-        <v>21</v>
-      </c>
       <c r="B23" s="0" t="s">
         <v>44</v>
       </c>
@@ -1253,9 +1187,6 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
-        <v>22</v>
-      </c>
       <c r="B24" s="0" t="s">
         <v>46</v>
       </c>
@@ -1264,9 +1195,6 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
-        <v>23</v>
-      </c>
       <c r="B25" s="0" t="s">
         <v>48</v>
       </c>
@@ -1275,9 +1203,6 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
-        <v>24</v>
-      </c>
       <c r="B26" s="0" t="s">
         <v>50</v>
       </c>
@@ -1286,9 +1211,6 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
-        <v>25</v>
-      </c>
       <c r="B27" s="0" t="s">
         <v>52</v>
       </c>
@@ -1297,9 +1219,6 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
-        <v>26</v>
-      </c>
       <c r="B28" s="0" t="s">
         <v>54</v>
       </c>
@@ -1308,9 +1227,6 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
-        <v>27</v>
-      </c>
       <c r="B29" s="0" t="s">
         <v>56</v>
       </c>
@@ -1319,9 +1235,6 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
-        <v>28</v>
-      </c>
       <c r="B30" s="0" t="s">
         <v>58</v>
       </c>
@@ -1330,9 +1243,6 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
-        <v>29</v>
-      </c>
       <c r="B31" s="0" t="s">
         <v>60</v>
       </c>
@@ -1341,9 +1251,6 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
-        <v>30</v>
-      </c>
       <c r="B32" s="0" t="s">
         <v>62</v>
       </c>
@@ -1352,9 +1259,6 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
-        <v>31</v>
-      </c>
       <c r="B33" s="0" t="s">
         <v>64</v>
       </c>
@@ -1363,9 +1267,6 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="n">
-        <v>32</v>
-      </c>
       <c r="B34" s="0" t="s">
         <v>66</v>
       </c>
@@ -1374,9 +1275,6 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="n">
-        <v>33</v>
-      </c>
       <c r="B35" s="0" t="s">
         <v>68</v>
       </c>
@@ -1385,9 +1283,6 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="n">
-        <v>34</v>
-      </c>
       <c r="B36" s="0" t="s">
         <v>70</v>
       </c>
@@ -1396,9 +1291,6 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="n">
-        <v>35</v>
-      </c>
       <c r="B37" s="0" t="s">
         <v>72</v>
       </c>
@@ -1407,9 +1299,6 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="n">
-        <v>36</v>
-      </c>
       <c r="B38" s="0" t="s">
         <v>74</v>
       </c>
@@ -1418,9 +1307,6 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="n">
-        <v>37</v>
-      </c>
       <c r="B39" s="0" t="s">
         <v>76</v>
       </c>
@@ -1429,9 +1315,6 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="n">
-        <v>38</v>
-      </c>
       <c r="B40" s="0" t="s">
         <v>78</v>
       </c>
@@ -1440,9 +1323,6 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="n">
-        <v>39</v>
-      </c>
       <c r="B41" s="0" t="s">
         <v>80</v>
       </c>
@@ -1451,9 +1331,6 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="n">
-        <v>40</v>
-      </c>
       <c r="B42" s="0" t="s">
         <v>82</v>
       </c>
@@ -1462,9 +1339,6 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="n">
-        <v>41</v>
-      </c>
       <c r="B43" s="0" t="s">
         <v>84</v>
       </c>
@@ -1473,9 +1347,6 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="n">
-        <v>42</v>
-      </c>
       <c r="B44" s="0" t="s">
         <v>86</v>
       </c>
@@ -1484,9 +1355,6 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="n">
-        <v>43</v>
-      </c>
       <c r="B45" s="0" t="s">
         <v>88</v>
       </c>
@@ -1495,9 +1363,6 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="n">
-        <v>44</v>
-      </c>
       <c r="B46" s="0" t="s">
         <v>90</v>
       </c>
@@ -1506,9 +1371,6 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="n">
-        <v>45</v>
-      </c>
       <c r="B47" s="0" t="s">
         <v>92</v>
       </c>
@@ -1517,9 +1379,6 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="n">
-        <v>46</v>
-      </c>
       <c r="B48" s="0" t="s">
         <v>94</v>
       </c>
@@ -1528,9 +1387,6 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="n">
-        <v>47</v>
-      </c>
       <c r="B49" s="0" t="s">
         <v>96</v>
       </c>
@@ -1539,9 +1395,6 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="n">
-        <v>48</v>
-      </c>
       <c r="B50" s="0" t="s">
         <v>98</v>
       </c>
@@ -1550,9 +1403,6 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="n">
-        <v>49</v>
-      </c>
       <c r="B51" s="0" t="s">
         <v>100</v>
       </c>
@@ -1561,9 +1411,6 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="n">
-        <v>50</v>
-      </c>
       <c r="B52" s="0" t="s">
         <v>102</v>
       </c>
@@ -1572,9 +1419,6 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="n">
-        <v>51</v>
-      </c>
       <c r="B53" s="0" t="s">
         <v>104</v>
       </c>
@@ -1583,9 +1427,6 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="n">
-        <v>52</v>
-      </c>
       <c r="B54" s="0" t="s">
         <v>106</v>
       </c>
@@ -1594,9 +1435,6 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="n">
-        <v>53</v>
-      </c>
       <c r="B55" s="0" t="s">
         <v>108</v>
       </c>
@@ -1605,9 +1443,6 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="n">
-        <v>54</v>
-      </c>
       <c r="B56" s="0" t="s">
         <v>110</v>
       </c>
@@ -1616,9 +1451,6 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="n">
-        <v>55</v>
-      </c>
       <c r="B57" s="0" t="s">
         <v>112</v>
       </c>
@@ -1627,9 +1459,6 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="n">
-        <v>56</v>
-      </c>
       <c r="B58" s="0" t="s">
         <v>114</v>
       </c>
@@ -1638,9 +1467,6 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="n">
-        <v>57</v>
-      </c>
       <c r="B59" s="0" t="s">
         <v>116</v>
       </c>
@@ -1649,9 +1475,6 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="n">
-        <v>58</v>
-      </c>
       <c r="B60" s="0" t="s">
         <v>118</v>
       </c>
@@ -1660,9 +1483,6 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="n">
-        <v>59</v>
-      </c>
       <c r="B61" s="0" t="s">
         <v>120</v>
       </c>
@@ -1671,9 +1491,6 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="n">
-        <v>60</v>
-      </c>
       <c r="B62" s="0" t="s">
         <v>122</v>
       </c>
@@ -1682,9 +1499,6 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="n">
-        <v>61</v>
-      </c>
       <c r="B63" s="0" t="s">
         <v>124</v>
       </c>
@@ -1693,9 +1507,6 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="n">
-        <v>62</v>
-      </c>
       <c r="B64" s="0" t="s">
         <v>126</v>
       </c>
@@ -1704,9 +1515,6 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="n">
-        <v>63</v>
-      </c>
       <c r="B65" s="0" t="s">
         <v>128</v>
       </c>
@@ -1715,9 +1523,6 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="n">
-        <v>64</v>
-      </c>
       <c r="B66" s="0" t="s">
         <v>130</v>
       </c>
@@ -1726,9 +1531,6 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="n">
-        <v>65</v>
-      </c>
       <c r="B67" s="0" t="s">
         <v>132</v>
       </c>
@@ -1737,9 +1539,6 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="n">
-        <v>66</v>
-      </c>
       <c r="B68" s="0" t="s">
         <v>134</v>
       </c>
@@ -1748,9 +1547,6 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="n">
-        <v>67</v>
-      </c>
       <c r="B69" s="0" t="s">
         <v>136</v>
       </c>
@@ -1759,9 +1555,6 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="n">
-        <v>68</v>
-      </c>
       <c r="B70" s="0" t="s">
         <v>138</v>
       </c>
@@ -1770,9 +1563,6 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="n">
-        <v>69</v>
-      </c>
       <c r="B71" s="0" t="s">
         <v>140</v>
       </c>
@@ -1781,9 +1571,6 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="n">
-        <v>70</v>
-      </c>
       <c r="B72" s="0" t="s">
         <v>142</v>
       </c>
@@ -1792,9 +1579,6 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="n">
-        <v>71</v>
-      </c>
       <c r="B73" s="0" t="s">
         <v>144</v>
       </c>
@@ -1803,9 +1587,6 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="n">
-        <v>72</v>
-      </c>
       <c r="B74" s="0" t="s">
         <v>146</v>
       </c>
@@ -1814,9 +1595,6 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="n">
-        <v>73</v>
-      </c>
       <c r="B75" s="0" t="s">
         <v>148</v>
       </c>
@@ -1825,9 +1603,6 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="n">
-        <v>74</v>
-      </c>
       <c r="B76" s="0" t="s">
         <v>150</v>
       </c>
@@ -1836,9 +1611,6 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="n">
-        <v>75</v>
-      </c>
       <c r="B77" s="0" t="s">
         <v>152</v>
       </c>
@@ -1847,9 +1619,6 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="n">
-        <v>76</v>
-      </c>
       <c r="B78" s="0" t="s">
         <v>154</v>
       </c>
@@ -1858,9 +1627,6 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="n">
-        <v>77</v>
-      </c>
       <c r="B79" s="0" t="s">
         <v>156</v>
       </c>
@@ -1869,9 +1635,6 @@
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="n">
-        <v>78</v>
-      </c>
       <c r="B80" s="0" t="s">
         <v>158</v>
       </c>
@@ -1880,9 +1643,6 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="n">
-        <v>79</v>
-      </c>
       <c r="B81" s="0" t="s">
         <v>160</v>
       </c>
@@ -1891,9 +1651,6 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="n">
-        <v>80</v>
-      </c>
       <c r="B82" s="0" t="s">
         <v>162</v>
       </c>
@@ -1902,9 +1659,6 @@
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="n">
-        <v>81</v>
-      </c>
       <c r="B83" s="0" t="s">
         <v>164</v>
       </c>
@@ -1913,9 +1667,6 @@
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="n">
-        <v>82</v>
-      </c>
       <c r="B84" s="0" t="s">
         <v>166</v>
       </c>
@@ -1924,9 +1675,6 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="n">
-        <v>83</v>
-      </c>
       <c r="B85" s="0" t="s">
         <v>168</v>
       </c>
@@ -1935,9 +1683,6 @@
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="n">
-        <v>84</v>
-      </c>
       <c r="B86" s="0" t="s">
         <v>170</v>
       </c>
@@ -1946,9 +1691,6 @@
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="n">
-        <v>85</v>
-      </c>
       <c r="B87" s="0" t="s">
         <v>172</v>
       </c>
@@ -1957,9 +1699,6 @@
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="n">
-        <v>86</v>
-      </c>
       <c r="B88" s="0" t="s">
         <v>174</v>
       </c>
@@ -1968,9 +1707,6 @@
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="n">
-        <v>87</v>
-      </c>
       <c r="B89" s="0" t="s">
         <v>176</v>
       </c>
@@ -1979,9 +1715,6 @@
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="n">
-        <v>88</v>
-      </c>
       <c r="B90" s="0" t="s">
         <v>178</v>
       </c>
@@ -1990,9 +1723,6 @@
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="n">
-        <v>89</v>
-      </c>
       <c r="B91" s="0" t="s">
         <v>180</v>
       </c>
@@ -2001,9 +1731,6 @@
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="n">
-        <v>90</v>
-      </c>
       <c r="B92" s="0" t="s">
         <v>182</v>
       </c>
@@ -2012,9 +1739,6 @@
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="n">
-        <v>91</v>
-      </c>
       <c r="B93" s="0" t="s">
         <v>184</v>
       </c>
@@ -2023,9 +1747,6 @@
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0" t="n">
-        <v>92</v>
-      </c>
       <c r="B94" s="0" t="s">
         <v>186</v>
       </c>
@@ -2034,9 +1755,6 @@
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0" t="n">
-        <v>93</v>
-      </c>
       <c r="B95" s="0" t="s">
         <v>188</v>
       </c>
@@ -2045,9 +1763,6 @@
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="0" t="n">
-        <v>94</v>
-      </c>
       <c r="B96" s="0" t="s">
         <v>190</v>
       </c>
@@ -2056,9 +1771,6 @@
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="0" t="n">
-        <v>95</v>
-      </c>
       <c r="B97" s="0" t="s">
         <v>192</v>
       </c>
@@ -2067,9 +1779,6 @@
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="0" t="n">
-        <v>96</v>
-      </c>
       <c r="B98" s="0" t="s">
         <v>194</v>
       </c>
@@ -2078,9 +1787,6 @@
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="n">
-        <v>97</v>
-      </c>
       <c r="B99" s="0" t="s">
         <v>196</v>
       </c>
@@ -2089,9 +1795,6 @@
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="0" t="n">
-        <v>98</v>
-      </c>
       <c r="B100" s="0" t="s">
         <v>198</v>
       </c>
@@ -2100,9 +1803,6 @@
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="0" t="n">
-        <v>99</v>
-      </c>
       <c r="B101" s="0" t="s">
         <v>200</v>
       </c>
@@ -2111,9 +1811,6 @@
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0" t="n">
-        <v>100</v>
-      </c>
       <c r="B102" s="0" t="s">
         <v>202</v>
       </c>
@@ -2122,9 +1819,6 @@
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="0" t="n">
-        <v>101</v>
-      </c>
       <c r="B103" s="0" t="s">
         <v>204</v>
       </c>
@@ -2133,9 +1827,6 @@
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0" t="n">
-        <v>102</v>
-      </c>
       <c r="B104" s="0" t="s">
         <v>206</v>
       </c>
@@ -2144,9 +1835,6 @@
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="0" t="n">
-        <v>103</v>
-      </c>
       <c r="B105" s="0" t="s">
         <v>208</v>
       </c>
@@ -2155,9 +1843,6 @@
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="0" t="n">
-        <v>104</v>
-      </c>
       <c r="B106" s="0" t="s">
         <v>210</v>
       </c>
@@ -2166,9 +1851,6 @@
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="0" t="n">
-        <v>105</v>
-      </c>
       <c r="B107" s="0" t="s">
         <v>212</v>
       </c>
@@ -2177,9 +1859,6 @@
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="0" t="n">
-        <v>106</v>
-      </c>
       <c r="B108" s="0" t="s">
         <v>214</v>
       </c>
@@ -2188,9 +1867,6 @@
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="0" t="n">
-        <v>107</v>
-      </c>
       <c r="B109" s="0" t="s">
         <v>216</v>
       </c>
@@ -2199,9 +1875,6 @@
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="0" t="n">
-        <v>108</v>
-      </c>
       <c r="B110" s="0" t="s">
         <v>218</v>
       </c>
@@ -2210,9 +1883,6 @@
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="0" t="n">
-        <v>109</v>
-      </c>
       <c r="B111" s="0" t="s">
         <v>220</v>
       </c>
@@ -2221,9 +1891,6 @@
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="0" t="n">
-        <v>110</v>
-      </c>
       <c r="B112" s="0" t="s">
         <v>222</v>
       </c>
@@ -2232,9 +1899,6 @@
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="0" t="n">
-        <v>111</v>
-      </c>
       <c r="B113" s="0" t="s">
         <v>224</v>
       </c>
@@ -2243,9 +1907,6 @@
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="0" t="n">
-        <v>112</v>
-      </c>
       <c r="B114" s="0" t="s">
         <v>226</v>
       </c>
@@ -2254,9 +1915,6 @@
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="0" t="n">
-        <v>113</v>
-      </c>
       <c r="B115" s="0" t="s">
         <v>228</v>
       </c>
@@ -2265,9 +1923,6 @@
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="0" t="n">
-        <v>114</v>
-      </c>
       <c r="B116" s="0" t="s">
         <v>230</v>
       </c>
@@ -2276,9 +1931,6 @@
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="0" t="n">
-        <v>115</v>
-      </c>
       <c r="B117" s="0" t="s">
         <v>232</v>
       </c>
@@ -2287,9 +1939,6 @@
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="0" t="n">
-        <v>116</v>
-      </c>
       <c r="B118" s="0" t="s">
         <v>234</v>
       </c>
@@ -2298,9 +1947,6 @@
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="0" t="n">
-        <v>117</v>
-      </c>
       <c r="B119" s="0" t="s">
         <v>236</v>
       </c>
@@ -2309,9 +1955,6 @@
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="0" t="n">
-        <v>118</v>
-      </c>
       <c r="B120" s="0" t="s">
         <v>238</v>
       </c>
@@ -2320,9 +1963,6 @@
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="0" t="n">
-        <v>119</v>
-      </c>
       <c r="B121" s="0" t="s">
         <v>240</v>
       </c>
@@ -2331,9 +1971,6 @@
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="0" t="n">
-        <v>120</v>
-      </c>
       <c r="B122" s="0" t="s">
         <v>242</v>
       </c>
@@ -2342,9 +1979,6 @@
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="0" t="n">
-        <v>121</v>
-      </c>
       <c r="B123" s="0" t="s">
         <v>244</v>
       </c>
@@ -2353,9 +1987,6 @@
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="0" t="n">
-        <v>122</v>
-      </c>
       <c r="B124" s="0" t="s">
         <v>246</v>
       </c>
@@ -2364,9 +1995,6 @@
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="0" t="n">
-        <v>123</v>
-      </c>
       <c r="B125" s="0" t="s">
         <v>248</v>
       </c>
@@ -2375,9 +2003,6 @@
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="0" t="n">
-        <v>124</v>
-      </c>
       <c r="B126" s="0" t="s">
         <v>250</v>
       </c>
@@ -2386,9 +2011,6 @@
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="0" t="n">
-        <v>125</v>
-      </c>
       <c r="B127" s="0" t="s">
         <v>252</v>
       </c>
@@ -2397,9 +2019,6 @@
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="0" t="n">
-        <v>126</v>
-      </c>
       <c r="B128" s="0" t="s">
         <v>254</v>
       </c>
@@ -2408,9 +2027,6 @@
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="0" t="n">
-        <v>127</v>
-      </c>
       <c r="B129" s="0" t="s">
         <v>256</v>
       </c>
@@ -2419,9 +2035,6 @@
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="0" t="n">
-        <v>128</v>
-      </c>
       <c r="B130" s="0" t="s">
         <v>258</v>
       </c>
@@ -2430,9 +2043,6 @@
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="0" t="n">
-        <v>129</v>
-      </c>
       <c r="B131" s="0" t="s">
         <v>260</v>
       </c>
@@ -2441,9 +2051,6 @@
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="0" t="n">
-        <v>130</v>
-      </c>
       <c r="B132" s="0" t="s">
         <v>262</v>
       </c>
@@ -2452,9 +2059,6 @@
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="0" t="n">
-        <v>131</v>
-      </c>
       <c r="B133" s="0" t="s">
         <v>264</v>
       </c>
@@ -2463,9 +2067,6 @@
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="0" t="n">
-        <v>132</v>
-      </c>
       <c r="B134" s="0" t="s">
         <v>266</v>
       </c>
@@ -2474,9 +2075,6 @@
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="0" t="n">
-        <v>133</v>
-      </c>
       <c r="B135" s="0" t="s">
         <v>268</v>
       </c>
@@ -2485,9 +2083,6 @@
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="0" t="n">
-        <v>134</v>
-      </c>
       <c r="B136" s="0" t="s">
         <v>270</v>
       </c>
@@ -2496,9 +2091,6 @@
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="0" t="n">
-        <v>135</v>
-      </c>
       <c r="B137" s="0" t="s">
         <v>272</v>
       </c>
@@ -2507,9 +2099,6 @@
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="0" t="n">
-        <v>136</v>
-      </c>
       <c r="B138" s="0" t="s">
         <v>274</v>
       </c>
@@ -2518,9 +2107,6 @@
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="0" t="n">
-        <v>137</v>
-      </c>
       <c r="B139" s="0" t="s">
         <v>276</v>
       </c>
@@ -2529,9 +2115,6 @@
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="0" t="n">
-        <v>138</v>
-      </c>
       <c r="B140" s="0" t="s">
         <v>278</v>
       </c>
@@ -2540,9 +2123,6 @@
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="0" t="n">
-        <v>139</v>
-      </c>
       <c r="B141" s="0" t="s">
         <v>280</v>
       </c>
@@ -2551,9 +2131,6 @@
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="0" t="n">
-        <v>140</v>
-      </c>
       <c r="B142" s="0" t="s">
         <v>282</v>
       </c>

</xml_diff>